<commit_message>
Modification de couleur de exel
</commit_message>
<xml_diff>
--- a/donnees.xlsx
+++ b/donnees.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +25,25 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00551585"/>
+        <bgColor rgb="00551585"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +51,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,229 +439,229 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>CT_NUM</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>CT_INTITULE</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>SUMS</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>CZ22003</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>COATS</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>-8268130.86</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>CZ22010</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>VINTANA TEXTILE</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2" t="n">
         <v>9022687.689999999</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>C22002</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>FESTIVAL SA</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2" t="n">
         <v>6315092</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>CZ22023</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>HARDY HENRI TEXTILES MADA SA</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="2" t="n">
         <v>392428.58</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>CZ22022</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">SUPRA KNITS </t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="2" t="n">
         <v>1293600</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>CZ22008</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>GENERAL GARNEMENT</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="2" t="n">
         <v>6510878.01</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>CZ22011</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>MIKEO KNITS</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="2" t="n">
         <v>225437.11</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>F22014</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>SAHAM</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="2" t="n">
         <v>-602977.5</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>F22022</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>MAZARS FIVOARANA</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>CZ22017</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>GAMA TEXTILE MADAGASCAR</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>C22001</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>SMTP</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>CZ22019</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>FOCUS TEXTILES</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="2" t="n">
         <v>3257266.49</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>CZ22012</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>ARAWAK SA</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="2" t="n">
         <v>3698839.6</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>F22024</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>AGRIKOBA</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="2" t="n">
         <v>-23875.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rectificaion de l'envoi bloquant email
</commit_message>
<xml_diff>
--- a/donnees.xlsx
+++ b/donnees.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>